<commit_message>
fix: new A11.五岁以下死亡监测(季度) DeathMonitorUnder5QuarterlyArea
</commit_message>
<xml_diff>
--- a/VL.Research/XMLConfig/DeathMonitorUnder5QuarterlyArea/5岁以下儿童死亡监测表.xlsx
+++ b/VL.Research/XMLConfig/DeathMonitorUnder5QuarterlyArea/5岁以下儿童死亡监测表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21480" windowHeight="12990"/>
+    <workbookView windowWidth="21000" windowHeight="11820"/>
   </bookViews>
   <sheets>
     <sheet name="列表" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
   <si>
     <t>5岁以下儿童死亡监测表</t>
   </si>
@@ -394,9 +394,6 @@
   </si>
   <si>
     <t>@LoopAuto_Data_wusuiswother</t>
-  </si>
-  <si>
-    <t xml:space="preserve">填报单位    </t>
   </si>
   <si>
     <t>@DataUser_FuWuJGMC</t>
@@ -467,10 +464,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="35">
     <font>
@@ -542,12 +539,42 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -555,8 +582,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -571,23 +614,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -617,13 +644,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -632,23 +652,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -671,15 +676,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -718,19 +715,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -742,97 +871,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -844,61 +889,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -985,23 +982,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1021,6 +1003,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1032,6 +1034,21 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1059,26 +1076,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1087,10 +1084,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1099,133 +1096,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
@@ -1288,10 +1285,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1939,7 +1936,7 @@
   <dimension ref="A1:Y17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="B3" sqref="B$1:C$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
@@ -2355,25 +2352,22 @@
       <c r="B11" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="I11" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="35" t="s">
+      <c r="J11" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="K11" s="24" t="s">
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="26"/>
+      <c r="S11" s="35" t="s">
         <v>42</v>
-      </c>
-      <c r="L11" s="24"/>
-      <c r="M11" s="24"/>
-      <c r="S11" s="35" t="s">
-        <v>43</v>
       </c>
       <c r="T11" s="35"/>
       <c r="U11" s="25"/>
@@ -2402,7 +2396,7 @@
     </row>
     <row r="13" s="2" customFormat="1" customHeight="1" spans="1:25">
       <c r="A13" s="27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B13" s="27"/>
       <c r="C13" s="27"/>
@@ -2431,7 +2425,7 @@
     </row>
     <row r="14" s="2" customFormat="1" spans="1:25">
       <c r="A14" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B14" s="27"/>
       <c r="C14" s="27"/>
@@ -2466,12 +2460,12 @@
     </row>
     <row r="16" s="2" customFormat="1" spans="1:1">
       <c r="A16" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" s="2" customFormat="1" spans="1:1">
       <c r="A17" s="30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -2489,8 +2483,8 @@
     <mergeCell ref="N7:Q7"/>
     <mergeCell ref="R7:U7"/>
     <mergeCell ref="V7:Y7"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="J11:L11"/>
     <mergeCell ref="S11:T11"/>
     <mergeCell ref="V11:X11"/>
     <mergeCell ref="A13:Y13"/>

</xml_diff>